<commit_message>
WIP : Getting Started Sample
</commit_message>
<xml_diff>
--- a/Examples/SpotTrading/SpotTrading/Views/FXSpotTrading.xlsx
+++ b/Examples/SpotTrading/SpotTrading/Views/FXSpotTrading.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="630" yWindow="-45" windowWidth="20565" windowHeight="9270"/>
   </bookViews>
   <sheets>
     <sheet name="Trading" sheetId="1" r:id="rId1"/>
-    <sheet name="Configuration" sheetId="2" r:id="rId2"/>
+    <sheet name="Data" sheetId="3" r:id="rId2"/>
+    <sheet name="Configuration" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="ExcelMvc.Form.Deal">Configuration!$I$32:$N$37</definedName>
-    <definedName name="ExcelMvc.Table.CcyPairs">Configuration!$I$3:$N$7</definedName>
-    <definedName name="ExcelMvc.Table.Ccys">Configuration!$I$10:$N$12</definedName>
-    <definedName name="ExcelMvc.Table.Positions">Configuration!$I$23:$N$29</definedName>
-    <definedName name="ExcelMvc.Table.Rates">Configuration!$I$15:$N$20</definedName>
+    <definedName name="ExcelMvc.Form.Deal">Configuration!$A$32:$F$37</definedName>
+    <definedName name="ExcelMvc.Table.CcyPairs">Configuration!$A$3:$F$7</definedName>
+    <definedName name="ExcelMvc.Table.Ccys">Configuration!$A$10:$F$12</definedName>
+    <definedName name="ExcelMvc.Table.Positions">Configuration!$A$23:$F$29</definedName>
+    <definedName name="ExcelMvc.Table.Rates">Configuration!$A$15:$F$20</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="58">
   <si>
     <t>CCY1</t>
   </si>
@@ -138,9 +139,6 @@
     <t>End Cell</t>
   </si>
   <si>
-    <t>Currency Pair Positions</t>
-  </si>
-  <si>
     <t>Exchange Rates</t>
   </si>
   <si>
@@ -193,6 +191,12 @@
   </si>
   <si>
     <t>USD/HKD</t>
+  </si>
+  <si>
+    <t>Deal Form</t>
+  </si>
+  <si>
+    <t>Currency Positions</t>
   </si>
 </sst>
 </file>
@@ -364,6 +368,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -374,14 +381,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>12825</xdr:rowOff>
+      <xdr:rowOff>127125</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="ExcelMvcRunCommandAction" textlink="">
       <xdr:nvSpPr>
@@ -390,7 +397,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="990600" y="876300"/>
+          <a:off x="990600" y="990600"/>
           <a:ext cx="866775" cy="270000"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -452,15 +459,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>9523</xdr:rowOff>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>19048</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1057275</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>257175</xdr:rowOff>
+      <xdr:colOff>1076325</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="ExcelMvcRunCommandAction" textlink="">
       <xdr:nvSpPr>
@@ -469,7 +476,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2828925" y="200023"/>
+          <a:off x="2847975" y="400048"/>
           <a:ext cx="1019175" cy="533402"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -541,15 +548,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
+      <xdr:colOff>504825</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>2</xdr:rowOff>
+      <xdr:rowOff>171452</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="ExcelMvcRunCommandAction" textlink="">
       <xdr:nvSpPr>
@@ -558,7 +565,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7724775" y="1743075"/>
+          <a:off x="7753350" y="1914525"/>
           <a:ext cx="1019175" cy="533402"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -665,7 +672,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -700,7 +707,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -909,11 +916,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I119"/>
+  <dimension ref="A1:I120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M20" sqref="M20"/>
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,86 +934,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+    <row r="3" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="11"/>
-    </row>
-    <row r="3" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>6</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="11"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="5"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+    <row r="4" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="11"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="5"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="2">
+        <f>SUM(E10:E29)</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="2">
-        <f>SUM(E9:E28)</f>
+    </row>
+    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="G7" s="12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H8" s="3" t="s">
+      <c r="G9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="G9" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="H9" s="20">
-        <v>0.92</v>
-      </c>
-      <c r="I9" s="20">
-        <v>0.92</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1016,13 +1012,13 @@
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="G10" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H10" s="20">
-        <v>102.4</v>
+        <v>0.92</v>
       </c>
       <c r="I10" s="20">
-        <v>102.4</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1032,13 +1028,13 @@
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="G11" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H11" s="20">
-        <v>1.68</v>
+        <v>102.4</v>
       </c>
       <c r="I11" s="20">
-        <v>1.68</v>
+        <v>102.4</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1048,13 +1044,13 @@
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="G12" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H12" s="20">
-        <v>1.37</v>
+        <v>1.68</v>
       </c>
       <c r="I12" s="20">
-        <v>1.37</v>
+        <v>1.68</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1064,13 +1060,13 @@
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="G13" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H13" s="20">
-        <v>6.24</v>
+        <v>1.37</v>
       </c>
       <c r="I13" s="20">
-        <v>6.24</v>
+        <v>1.37</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1080,13 +1076,13 @@
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="G14" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H14" s="20">
-        <v>7.75</v>
+        <v>6.24</v>
       </c>
       <c r="I14" s="20">
-        <v>7.75</v>
+        <v>6.24</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1095,9 +1091,15 @@
       <c r="C15" s="7"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
+      <c r="G15" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H15" s="20">
+        <v>7.75</v>
+      </c>
+      <c r="I15" s="20">
+        <v>7.75</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
@@ -1229,8 +1231,18 @@
       <c r="H28" s="20"/>
       <c r="I28" s="20"/>
     </row>
-    <row r="119" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E119">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+    </row>
+    <row r="120" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E120">
         <v>333</v>
       </c>
     </row>
@@ -1243,44 +1255,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N37"/>
+  <dimension ref="A2:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.5703125" customWidth="1"/>
     <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="14"/>
     <col min="8" max="8" width="16.28515625" customWidth="1"/>
-    <col min="9" max="9" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" customWidth="1"/>
-    <col min="14" max="14" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" s="12"/>
       <c r="F2" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="15"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-    </row>
-    <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>0</v>
       </c>
@@ -1288,35 +1287,17 @@
         <v>2</v>
       </c>
       <c r="C3" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="19" t="s">
         <v>43</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>44</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="M3" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="N3" s="17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
@@ -1332,26 +1313,8 @@
       <c r="F4" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="6" t="str">
-        <f ca="1">CELL("address", A4)</f>
-        <v>$A$4</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6" t="str">
-        <f ca="1">CELL("address", A21)</f>
-        <v>$A$21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
@@ -1367,26 +1330,8 @@
       <c r="F5" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="6" t="str">
-        <f ca="1">CELL("address", B4)</f>
-        <v>$B$4</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6" t="str">
-        <f ca="1">CELL("address", B21)</f>
-        <v>$B$21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>13</v>
       </c>
@@ -1402,26 +1347,8 @@
       <c r="F6" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="6" t="str">
-        <f ca="1">CELL("address", C4)</f>
-        <v>$C$4</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6" t="str">
-        <f ca="1">CELL("address", C21)</f>
-        <v>$C$21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>14</v>
       </c>
@@ -1437,26 +1364,8 @@
       <c r="F7" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="6" t="str">
-        <f ca="1">CELL("address", D4)</f>
-        <v>$D$4</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6" t="str">
-        <f ca="1">CELL("address", D21)</f>
-        <v>$D$21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>11</v>
       </c>
@@ -1473,7 +1382,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
@@ -1489,16 +1398,8 @@
       <c r="F9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="J9" s="15"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-    </row>
-    <row r="10" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -1506,438 +1407,607 @@
       <c r="F10" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="I10" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="J10" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="K10" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="L10" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="M10" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="N10" s="17" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
-      <c r="I11" s="6" t="str">
-        <f ca="1">CELL("address", F4)</f>
-        <v>$F$4</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L11" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
-      <c r="I14" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="J14" s="15"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="16"/>
-      <c r="N14" s="16"/>
-    </row>
-    <row r="15" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
-      <c r="I15" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="J15" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="K15" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="L15" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="M15" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="N15" s="17" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
-      <c r="I16" s="6" t="str">
-        <f ca="1">CELL("address", Trading!G9)</f>
-        <v>[FXSpotTrading.xlsx]Trading!$G$9</v>
-      </c>
-      <c r="J16" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="K16" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L16" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
-      <c r="I18" s="6" t="str">
-        <f ca="1">CELL("address",Trading!H9)</f>
-        <v>[FXSpotTrading.xlsx]Trading!$H$9</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="K18" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L18" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
-      <c r="I19" s="6" t="str">
-        <f ca="1">CELL("address", Trading!I9)</f>
-        <v>[FXSpotTrading.xlsx]Trading!$I$9</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="K19" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L19" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>46</v>
       </c>
-      <c r="I22" s="15" t="s">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:F37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="59" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="str">
+        <f ca="1">CELL("address", Data!A4)</f>
+        <v>[FXSpotTrading.xlsx]Data!$A$4</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6" t="str">
+        <f ca="1">CELL("address", Data!A21)</f>
+        <v>[FXSpotTrading.xlsx]Data!$A$21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="str">
+        <f ca="1">CELL("address", Data!B4)</f>
+        <v>[FXSpotTrading.xlsx]Data!$B$4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6" t="str">
+        <f ca="1">CELL("address", Data!B21)</f>
+        <v>[FXSpotTrading.xlsx]Data!$B$21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="str">
+        <f ca="1">CELL("address", Data!C4)</f>
+        <v>[FXSpotTrading.xlsx]Data!$C$4</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6" t="str">
+        <f ca="1">CELL("address", Data!C21)</f>
+        <v>[FXSpotTrading.xlsx]Data!$C$21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="str">
+        <f ca="1">CELL("address", Data!D4)</f>
+        <v>[FXSpotTrading.xlsx]Data!$D$4</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6" t="str">
+        <f ca="1">CELL("address", Data!D21)</f>
+        <v>[FXSpotTrading.xlsx]Data!$D$21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="15"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="str">
+        <f ca="1">CELL("address", Data!F4)</f>
+        <v>[FXSpotTrading.xlsx]Data!$F$4</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="str">
+        <f ca="1">CELL("address", Trading!G10)</f>
+        <v>[FXSpotTrading.xlsx]Trading!$G$10</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="str">
+        <f ca="1">CELL("address",Trading!H10)</f>
+        <v>[FXSpotTrading.xlsx]Trading!$H$10</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="str">
+        <f ca="1">CELL("address", Trading!I10)</f>
+        <v>[FXSpotTrading.xlsx]Trading!$I$10</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="J22" s="15"/>
-      <c r="K22" s="16"/>
-      <c r="L22" s="16"/>
-      <c r="M22" s="16"/>
-      <c r="N22" s="16"/>
-    </row>
-    <row r="23" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>47</v>
-      </c>
-      <c r="I23" s="17" t="s">
+      <c r="B22" s="15"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="J23" s="17" t="s">
+      <c r="B23" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="K23" s="17" t="s">
+      <c r="C23" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="L23" s="17" t="s">
+      <c r="D23" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="M23" s="17" t="s">
+      <c r="E23" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="N23" s="17" t="s">
+      <c r="F23" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>45</v>
-      </c>
-      <c r="I24" s="6" t="str">
-        <f ca="1">CELL("address", Trading!A9)</f>
-        <v>[FXSpotTrading.xlsx]Trading!$A$9</v>
-      </c>
-      <c r="J24" s="6" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="str">
+        <f ca="1">CELL("address", Trading!A10)</f>
+        <v>[FXSpotTrading.xlsx]Trading!$A$10</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="K24" s="6" t="s">
+      <c r="C24" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="L24" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="M24" s="6"/>
-      <c r="N24" s="6"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I25" s="6" t="str">
-        <f ca="1">CELL("address", Trading!B9)</f>
-        <v>[FXSpotTrading.xlsx]Trading!$B$9</v>
-      </c>
-      <c r="J25" s="6" t="s">
+      <c r="D24" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="str">
+        <f ca="1">CELL("address", Trading!B10)</f>
+        <v>[FXSpotTrading.xlsx]Trading!$B$10</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="K25" s="6" t="s">
+      <c r="C25" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="L25" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="M25" s="6"/>
-      <c r="N25" s="6"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I26" s="6" t="str">
-        <f ca="1">CELL("address", Trading!C9)</f>
-        <v>[FXSpotTrading.xlsx]Trading!$C$9</v>
-      </c>
-      <c r="J26" s="6" t="s">
+      <c r="D25" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="str">
+        <f ca="1">CELL("address", Trading!C10)</f>
+        <v>[FXSpotTrading.xlsx]Trading!$C$10</v>
+      </c>
+      <c r="B26" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="K26" s="6" t="s">
+      <c r="C26" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="L26" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="M26" s="6"/>
-      <c r="N26" s="6"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I27" s="6" t="str">
-        <f ca="1">CELL("address", Trading!D9)</f>
-        <v>[FXSpotTrading.xlsx]Trading!$D$9</v>
-      </c>
-      <c r="J27" s="6" t="s">
+      <c r="D26" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="str">
+        <f ca="1">CELL("address", Trading!D10)</f>
+        <v>[FXSpotTrading.xlsx]Trading!$D$10</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="K27" s="6" t="s">
+      <c r="C27" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="L27" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="M27" s="6"/>
-      <c r="N27" s="6"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I28" s="6" t="str">
-        <f ca="1">CELL("address", Trading!E9)</f>
-        <v>[FXSpotTrading.xlsx]Trading!$E$9</v>
-      </c>
-      <c r="J28" s="6" t="s">
+      <c r="D27" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="str">
+        <f ca="1">CELL("address", Trading!E10)</f>
+        <v>[FXSpotTrading.xlsx]Trading!$E$10</v>
+      </c>
+      <c r="B28" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="K28" s="6" t="s">
+      <c r="C28" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="L28" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="M28" s="6"/>
-      <c r="N28" s="6"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
-      <c r="M29" s="6"/>
-      <c r="N29" s="6"/>
-    </row>
-    <row r="31" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="I31" s="15" t="s">
+      <c r="D28" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="J31" s="15"/>
-      <c r="K31" s="16"/>
-      <c r="L31" s="16"/>
-      <c r="M31" s="16"/>
-      <c r="N31" s="16"/>
-    </row>
-    <row r="32" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="I32" s="17" t="s">
+      <c r="B31" s="15"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="J32" s="17" t="s">
+      <c r="B32" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="K32" s="17" t="s">
+      <c r="C32" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="L32" s="17" t="s">
+      <c r="D32" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="M32" s="17" t="s">
+      <c r="E32" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="N32" s="17" t="s">
+      <c r="F32" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I33" s="6" t="str">
-        <f ca="1">CELL("address",Trading!B2)</f>
-        <v>[FXSpotTrading.xlsx]Trading!$B$2</v>
-      </c>
-      <c r="J33" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="K33" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="L33" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="M33" s="6"/>
-      <c r="N33" s="6" t="str">
-        <f ca="1">CONCATENATE(CELL("address",F4), ":", CELL("address",F100))</f>
-        <v>$F$4:$F$100</v>
-      </c>
-    </row>
-    <row r="34" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I34" s="6" t="str">
-        <f ca="1">CELL("address",Trading!C2)</f>
-        <v>[FXSpotTrading.xlsx]Trading!$C$2</v>
-      </c>
-      <c r="J34" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="K34" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="L34" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="M34" s="6"/>
-      <c r="N34" s="6"/>
-    </row>
-    <row r="35" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I35" s="6" t="str">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="str">
         <f ca="1">CELL("address",Trading!B3)</f>
         <v>[FXSpotTrading.xlsx]Trading!$B$3</v>
       </c>
-      <c r="J35" s="6" t="s">
+      <c r="B33" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6" t="str">
+        <f ca="1">CONCATENATE(CELL("address", Data!F4), ":", CELL("address",Data!F100))</f>
+        <v>[FXSpotTrading.xlsx]Data!$F$4:[FXSpotTrading.xlsx]Data!$F$100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="str">
+        <f ca="1">CELL("address",Trading!C3)</f>
+        <v>[FXSpotTrading.xlsx]Trading!$C$3</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="str">
+        <f ca="1">CELL("address",Trading!B4)</f>
+        <v>[FXSpotTrading.xlsx]Trading!$B$4</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="K35" s="6" t="s">
+      <c r="C35" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="L35" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="M35" s="6"/>
-      <c r="N35" s="6" t="str">
-        <f ca="1">CONCATENATE(CELL("address",F4), ":", CELL("address",F100))</f>
-        <v>$F$4:$F$100</v>
-      </c>
-    </row>
-    <row r="36" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I36" s="6" t="str">
-        <f ca="1">CELL("address", Trading!C3)</f>
-        <v>[FXSpotTrading.xlsx]Trading!$C$3</v>
-      </c>
-      <c r="J36" s="6" t="s">
+      <c r="D35" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6" t="str">
+        <f ca="1">CONCATENATE(CELL("address", Data!F4), ":", CELL("address",Data!F100))</f>
+        <v>[FXSpotTrading.xlsx]Data!$F$4:[FXSpotTrading.xlsx]Data!$F$100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="str">
+        <f ca="1">CELL("address", Trading!C4)</f>
+        <v>[FXSpotTrading.xlsx]Trading!$C$4</v>
+      </c>
+      <c r="B36" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="K36" s="6" t="s">
+      <c r="C36" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="L36" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="M36" s="6"/>
-      <c r="N36" s="6"/>
-    </row>
-    <row r="37" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6"/>
-      <c r="M37" s="6"/>
-      <c r="N37" s="6"/>
+      <c r="D36" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
WIP : Trading Sample
</commit_message>
<xml_diff>
--- a/Examples/SpotTrading/SpotTrading/Views/FXSpotTrading.xlsx
+++ b/Examples/SpotTrading/SpotTrading/Views/FXSpotTrading.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="62">
   <si>
     <t>CCY1</t>
   </si>
@@ -197,6 +197,18 @@
   </si>
   <si>
     <t>Currency Positions</t>
+  </si>
+  <si>
+    <t>BuyCcy</t>
+  </si>
+  <si>
+    <t>SellCcy</t>
+  </si>
+  <si>
+    <t>BuyAmount</t>
+  </si>
+  <si>
+    <t>SellAmount</t>
   </si>
 </sst>
 </file>
@@ -324,10 +336,6 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -350,6 +358,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="40" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -920,7 +932,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N14" sqref="N14"/>
+      <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -934,7 +946,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>56</v>
       </c>
     </row>
@@ -951,21 +963,21 @@
         <v>5</v>
       </c>
       <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
+      <c r="C3" s="20"/>
     </row>
     <row r="4" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="10"/>
-      <c r="C4" s="11"/>
+      <c r="C4" s="20"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="11" t="s">
         <v>57</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -975,7 +987,7 @@
         <f>SUM(E10:E29)</f>
         <v>0</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="11" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1014,10 +1026,10 @@
       <c r="G10" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="H10" s="20">
+      <c r="H10" s="19">
         <v>0.92</v>
       </c>
-      <c r="I10" s="20">
+      <c r="I10" s="19">
         <v>0.92</v>
       </c>
     </row>
@@ -1030,10 +1042,10 @@
       <c r="G11" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="H11" s="20">
+      <c r="H11" s="19">
         <v>102.4</v>
       </c>
-      <c r="I11" s="20">
+      <c r="I11" s="19">
         <v>102.4</v>
       </c>
     </row>
@@ -1046,10 +1058,10 @@
       <c r="G12" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="H12" s="20">
+      <c r="H12" s="19">
         <v>1.68</v>
       </c>
-      <c r="I12" s="20">
+      <c r="I12" s="19">
         <v>1.68</v>
       </c>
     </row>
@@ -1062,10 +1074,10 @@
       <c r="G13" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="H13" s="20">
+      <c r="H13" s="19">
         <v>1.37</v>
       </c>
-      <c r="I13" s="20">
+      <c r="I13" s="19">
         <v>1.37</v>
       </c>
     </row>
@@ -1078,10 +1090,10 @@
       <c r="G14" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="H14" s="20">
+      <c r="H14" s="19">
         <v>6.24</v>
       </c>
-      <c r="I14" s="20">
+      <c r="I14" s="19">
         <v>6.24</v>
       </c>
     </row>
@@ -1094,10 +1106,10 @@
       <c r="G15" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H15" s="20">
+      <c r="H15" s="19">
         <v>7.75</v>
       </c>
-      <c r="I15" s="20">
+      <c r="I15" s="19">
         <v>7.75</v>
       </c>
     </row>
@@ -1108,8 +1120,8 @@
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="G16" s="6"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
@@ -1118,8 +1130,8 @@
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="G17" s="6"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
@@ -1128,8 +1140,8 @@
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="G18" s="6"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
@@ -1138,8 +1150,8 @@
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
@@ -1148,8 +1160,8 @@
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
@@ -1158,8 +1170,8 @@
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="G21" s="6"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
@@ -1168,8 +1180,8 @@
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="G22" s="6"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
@@ -1178,8 +1190,8 @@
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="G23" s="6"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
@@ -1188,8 +1200,8 @@
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="G24" s="6"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
@@ -1198,8 +1210,8 @@
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
       <c r="G25" s="6"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
@@ -1208,8 +1220,8 @@
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
       <c r="G26" s="6"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
@@ -1218,8 +1230,8 @@
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
       <c r="G27" s="6"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
@@ -1228,8 +1240,8 @@
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
       <c r="G28" s="6"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="20"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
@@ -1238,8 +1250,8 @@
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
       <c r="G29" s="6"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="20"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
     </row>
     <row r="120" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E120">
@@ -1266,30 +1278,30 @@
     <col min="1" max="1" width="8.5703125" customWidth="1"/>
     <col min="2" max="2" width="8.85546875" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="14"/>
+    <col min="6" max="6" width="9.140625" style="13"/>
     <col min="8" max="8" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="F2" s="13" t="s">
+      <c r="B2" s="11"/>
+      <c r="F2" s="12" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="18" t="s">
         <v>43</v>
       </c>
       <c r="E3" s="3"/>
@@ -1310,7 +1322,7 @@
       <c r="D4" s="6">
         <v>0.92</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="13" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1327,7 +1339,7 @@
       <c r="D5" s="6">
         <v>102.4</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="13" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1344,7 +1356,7 @@
       <c r="D6" s="6">
         <v>1.68</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="13" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1361,7 +1373,7 @@
       <c r="D7" s="6">
         <v>1.37</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="13" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1378,7 +1390,7 @@
       <c r="D8" s="6">
         <v>6.24</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="13" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1395,7 +1407,7 @@
       <c r="D9" s="6">
         <v>7.75</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="13" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1404,7 +1416,7 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="13" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1499,7 +1511,7 @@
   <dimension ref="A2:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1513,32 +1525,32 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="16" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1623,32 +1635,32 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="16" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1678,32 +1690,32 @@
       <c r="F12" s="6"/>
     </row>
     <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="F15" s="16" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1775,32 +1787,32 @@
       <c r="F20" s="6"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="D23" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E23" s="17" t="s">
+      <c r="E23" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="F23" s="17" t="s">
+      <c r="F23" s="16" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1898,32 +1910,32 @@
       <c r="F29" s="6"/>
     </row>
     <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="15" t="s">
+      <c r="A31" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="15"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
     </row>
     <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="17" t="s">
+      <c r="A32" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="C32" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D32" s="17" t="s">
+      <c r="D32" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E32" s="17" t="s">
+      <c r="E32" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="F32" s="17" t="s">
+      <c r="F32" s="16" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1933,7 +1945,7 @@
         <v>[FXSpotTrading.xlsx]Trading!$B$3</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>36</v>
@@ -1953,7 +1965,7 @@
         <v>[FXSpotTrading.xlsx]Trading!$C$3</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>36</v>
@@ -1970,7 +1982,7 @@
         <v>[FXSpotTrading.xlsx]Trading!$B$4</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>36</v>
@@ -1990,7 +2002,7 @@
         <v>[FXSpotTrading.xlsx]Trading!$C$4</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>36</v>

</xml_diff>